<commit_message>
0.0.6: Set null to telegram if no input/expect data specified.
</commit_message>
<xml_diff>
--- a/meta/test/00_GetTableSample.xlsx
+++ b/meta/test/00_GetTableSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B16004-D99C-8848-8724-71801405B874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4C1F27-2205-A244-BA3E-E57AAF6AD66B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="3860" windowWidth="26200" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="144">
   <si>
     <t>2.定義書様式に記入された情報から、メタファイルをXMLファイルに変換する処理の定義に相当するJavaソースコードが自動生成されます。</t>
   </si>
@@ -5690,8 +5690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2255131-13B1-484A-9393-AFEFC966B3D8}">
   <dimension ref="A1:Q143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L117" sqref="L117"/>
+    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -6925,24 +6925,12 @@
       <c r="K49" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="L49" s="84" t="s">
-        <v>33</v>
-      </c>
-      <c r="M49" s="180">
-        <v>500</v>
-      </c>
-      <c r="N49" s="180">
-        <v>30</v>
-      </c>
-      <c r="O49" s="180">
-        <v>50</v>
-      </c>
-      <c r="P49" s="180">
-        <v>100</v>
-      </c>
-      <c r="Q49" s="181" t="s">
-        <v>35</v>
-      </c>
+      <c r="L49" s="84"/>
+      <c r="M49" s="180"/>
+      <c r="N49" s="180"/>
+      <c r="O49" s="180"/>
+      <c r="P49" s="180"/>
+      <c r="Q49" s="181"/>
     </row>
     <row r="50" spans="1:17">
       <c r="A50" s="87">
@@ -6969,24 +6957,12 @@
       <c r="K50" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="L50" s="184" t="s">
-        <v>34</v>
-      </c>
-      <c r="M50" s="182">
-        <v>400</v>
-      </c>
-      <c r="N50" s="182">
-        <v>30</v>
-      </c>
-      <c r="O50" s="182">
-        <v>50</v>
-      </c>
-      <c r="P50" s="182">
-        <v>100</v>
-      </c>
-      <c r="Q50" s="183" t="s">
-        <v>35</v>
-      </c>
+      <c r="L50" s="184"/>
+      <c r="M50" s="182"/>
+      <c r="N50" s="182"/>
+      <c r="O50" s="182"/>
+      <c r="P50" s="182"/>
+      <c r="Q50" s="183"/>
     </row>
     <row r="51" spans="1:17">
       <c r="A51" s="87">
@@ -7013,24 +6989,12 @@
       <c r="K51" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="L51" s="184" t="s">
-        <v>36</v>
-      </c>
-      <c r="M51" s="184">
-        <v>300</v>
-      </c>
-      <c r="N51" s="182">
-        <v>30</v>
-      </c>
-      <c r="O51" s="182">
-        <v>50</v>
-      </c>
-      <c r="P51" s="182">
-        <v>100</v>
-      </c>
-      <c r="Q51" s="183" t="s">
-        <v>35</v>
-      </c>
+      <c r="L51" s="184"/>
+      <c r="M51" s="184"/>
+      <c r="N51" s="182"/>
+      <c r="O51" s="182"/>
+      <c r="P51" s="182"/>
+      <c r="Q51" s="183"/>
     </row>
     <row r="52" spans="1:17">
       <c r="A52" s="87">
@@ -7055,9 +7019,7 @@
       <c r="K52" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="L52" s="80" t="s">
-        <v>114</v>
-      </c>
+      <c r="L52" s="80"/>
       <c r="M52" s="80"/>
       <c r="N52" s="14"/>
       <c r="O52" s="14"/>

</xml_diff>